<commit_message>
Added 2 more entries to planes file fo tests, shows message when theres no connections, changed button text, prepared listview for data (it isn't connected yet)
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\OneDrive\Pulpit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia\SEM 6\RSO\WcfService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A92515F-5600-4E61-BA3E-2DDA0DABB76A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E927CB6-4C32-40A3-9D7B-76A5607B2DB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{222D3E1D-3C85-4B5F-8003-91E88CFCE22C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Starting City</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B4DD21-9861-47FE-9982-D41428DE8ED1}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,6 +445,34 @@
         <v>43970.767743055556</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43970.748611111114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43971.848611111112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43971.815972222219</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43972.640277777777</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>